<commit_message>
update illus mods generators
</commit_message>
<xml_diff>
--- a/MODS-DC-Generators/00 Illustrative-MODS-Generator-NEW/Illustrative-MODS-03.7.xlsx
+++ b/MODS-DC-Generators/00 Illustrative-MODS-Generator-NEW/Illustrative-MODS-03.7.xlsx
@@ -9240,9 +9240,6 @@
     <t>&amp;#169; Livingstone Spectral Imaging Project team. Creative Commons Attribution-NonCommercial 3.0 Unported (https://creativecommons.org/licenses/by-nc/3.0/).</t>
   </si>
   <si>
-    <t>Copyright Callum Bennetts - Maverick Photo Agency. Used by permission.</t>
-  </si>
-  <si>
     <t>Courtesy of Keith Boyer/Indiana University of Pennsylvania.</t>
   </si>
   <si>
@@ -9256,6 +9253,9 @@
   </si>
   <si>
     <t>Dr. Livingstone's Remains at Southampton; Procession to the Railway Station. Illustration from Illustrated London News (25 Apr. 1874)</t>
+  </si>
+  <si>
+    <t>&amp;#169; Callum Bennetts - Maverick Photo Agency. Used by permission.</t>
   </si>
 </sst>
 </file>
@@ -9376,7 +9376,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="802">
+  <cellStyleXfs count="804">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -9438,6 +9438,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -10360,7 +10362,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="802">
+  <cellStyles count="804">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -10770,6 +10772,7 @@
     <cellStyle name="Followed Hyperlink" xfId="797" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="799" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="801" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="803" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -11162,6 +11165,7 @@
     <cellStyle name="Hyperlink" xfId="796" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="798" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="800" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="802" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -11493,9 +11497,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P1109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A991" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B994" sqref="B994"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1025" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P1028" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -52359,10 +52363,10 @@
         <v>2645</v>
       </c>
       <c r="B994" s="9" t="s">
-        <v>3078</v>
+        <v>3077</v>
       </c>
       <c r="C994" s="9" t="s">
-        <v>3077</v>
+        <v>3076</v>
       </c>
       <c r="E994" s="9" t="s">
         <v>2900</v>
@@ -53825,7 +53829,7 @@
       <c r="M1029" s="37"/>
       <c r="N1029" s="37"/>
       <c r="P1029" s="28" t="s">
-        <v>3073</v>
+        <v>3078</v>
       </c>
     </row>
     <row r="1030" spans="1:16" ht="60">
@@ -53862,7 +53866,7 @@
       <c r="M1030" s="37"/>
       <c r="N1030" s="37"/>
       <c r="P1030" s="28" t="s">
-        <v>3073</v>
+        <v>3078</v>
       </c>
     </row>
     <row r="1031" spans="1:16" ht="45">
@@ -54401,7 +54405,7 @@
       <c r="M1044" s="37"/>
       <c r="N1044" s="37"/>
       <c r="P1044" s="28" t="s">
-        <v>3073</v>
+        <v>3078</v>
       </c>
     </row>
     <row r="1045" spans="1:16" ht="90">
@@ -54732,7 +54736,7 @@
       <c r="M1052" s="37"/>
       <c r="N1052" s="37"/>
       <c r="P1052" s="28" t="s">
-        <v>3073</v>
+        <v>3078</v>
       </c>
     </row>
     <row r="1053" spans="1:16" ht="45">
@@ -55005,7 +55009,7 @@
       <c r="M1059" s="37"/>
       <c r="N1059" s="37"/>
       <c r="P1059" s="28" t="s">
-        <v>3073</v>
+        <v>3078</v>
       </c>
     </row>
     <row r="1060" spans="1:16" ht="45">
@@ -55352,7 +55356,7 @@
       <c r="M1068" s="40"/>
       <c r="N1068" s="40"/>
       <c r="P1068" s="28" t="s">
-        <v>3074</v>
+        <v>3073</v>
       </c>
     </row>
     <row r="1069" spans="1:16" ht="45">
@@ -55389,7 +55393,7 @@
       <c r="M1069" s="37"/>
       <c r="N1069" s="37"/>
       <c r="P1069" s="28" t="s">
-        <v>3075</v>
+        <v>3074</v>
       </c>
     </row>
     <row r="1070" spans="1:16" ht="45">
@@ -55426,7 +55430,7 @@
       <c r="M1070" s="37"/>
       <c r="N1070" s="37"/>
       <c r="P1070" s="28" t="s">
-        <v>3076</v>
+        <v>3075</v>
       </c>
     </row>
     <row r="1071" spans="1:16" ht="75">

</xml_diff>